<commit_message>
calculate PWM for 0&180 degree, record the data in excel and the head of angle_cali.ino, rewrite the angletoPWM func
</commit_message>
<xml_diff>
--- a/tests/Motor/angle_cali.xlsx
+++ b/tests/Motor/angle_cali.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/M0riarty/Documents/LIMA/slimdog/tests/Motor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E5753F6C-3E72-2D45-B460-6547B562EF0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C75266B0-AB9C-DD4C-90BF-0A9E97968D22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19680" yWindow="2260" windowWidth="12360" windowHeight="12620" xr2:uid="{A629BED3-AD5C-924C-9DBB-2FB643719366}"/>
+    <workbookView xWindow="1740" yWindow="3840" windowWidth="12360" windowHeight="12620" xr2:uid="{A629BED3-AD5C-924C-9DBB-2FB643719366}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
   <si>
     <t>servo_id=4</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -122,6 +122,14 @@
   </si>
   <si>
     <t>Finally, calculate the corresponding smallest and greatest angles, and attach the behavior for easy understanding.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0degree</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>180degree</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -486,15 +494,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE68304C-707E-8545-B3E7-DCA0F147C5AD}">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="212" workbookViewId="0">
-      <selection activeCell="E5" sqref="E4:E5"/>
+    <sheetView tabSelected="1" topLeftCell="C29" zoomScale="137" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -502,17 +510,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:7">
       <c r="B2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:7">
       <c r="B3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -523,7 +531,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -536,8 +544,16 @@
       <c r="D5">
         <v>580</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="F5">
+        <f>C5-90*C4</f>
+        <v>130</v>
+      </c>
+      <c r="G5">
+        <f>C5+90*C4</f>
+        <v>670</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -552,8 +568,14 @@
         <f>90+(D5-C5)/3</f>
         <v>150</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -561,7 +583,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -570,7 +592,7 @@
         <v>2.6111111111111112</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:7">
       <c r="B10">
         <v>110</v>
       </c>
@@ -580,8 +602,16 @@
       <c r="D10">
         <v>470</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="F10">
+        <f>C10-90*C9</f>
+        <v>95</v>
+      </c>
+      <c r="G10">
+        <f>C10+90*C9</f>
+        <v>565</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="B11">
         <f>90+(B10-C10)/C9</f>
         <v>5.7446808510638334</v>
@@ -594,7 +624,7 @@
         <v>143.61702127659575</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:7">
       <c r="B12" t="s">
         <v>8</v>
       </c>
@@ -602,7 +632,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -611,7 +641,7 @@
         <v>3.0625</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:7">
       <c r="B14">
         <v>110</v>
       </c>
@@ -621,8 +651,16 @@
       <c r="D14">
         <v>590</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="F14">
+        <f>C14-90*C13</f>
+        <v>69.375</v>
+      </c>
+      <c r="G14">
+        <f>C14+90*C13</f>
+        <v>620.625</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="B15">
         <f>90+(B14-C14)/C13</f>
         <v>13.265306122448976</v>
@@ -635,7 +673,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:7">
       <c r="B16" t="s">
         <v>11</v>
       </c>
@@ -643,7 +681,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -652,7 +690,7 @@
         <v>3.333333333333333</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:7">
       <c r="B19">
         <v>140</v>
       </c>
@@ -662,8 +700,16 @@
       <c r="D19">
         <v>550</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="F19">
+        <f>C19-90*C18</f>
+        <v>80</v>
+      </c>
+      <c r="G19">
+        <f>C19+90*C18</f>
+        <v>680</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="B20">
         <f>90+(B19-C19)/C18</f>
         <v>18</v>
@@ -676,7 +722,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:7">
       <c r="B21" t="s">
         <v>4</v>
       </c>
@@ -684,7 +730,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -693,7 +739,7 @@
         <v>2.666666666666667</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:7">
       <c r="B23">
         <v>280</v>
       </c>
@@ -703,8 +749,16 @@
       <c r="D23">
         <v>680</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="F23">
+        <f>C23-90*C22</f>
+        <v>325</v>
+      </c>
+      <c r="G23">
+        <f>C23+90*C22</f>
+        <v>805</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="B24">
         <f>90+(B23-C23)/C22</f>
         <v>-16.874999999999986</v>
@@ -717,7 +771,7 @@
         <v>133.125</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:7">
       <c r="B25" t="s">
         <v>8</v>
       </c>
@@ -725,7 +779,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -734,7 +788,7 @@
         <v>2.6666666666666665</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:7">
       <c r="B27">
         <v>140</v>
       </c>
@@ -744,8 +798,16 @@
       <c r="D27">
         <v>660</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="F27">
+        <f>C27-90*C26</f>
+        <v>150</v>
+      </c>
+      <c r="G27">
+        <f>C27+90*C26</f>
+        <v>630</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="B28">
         <f>90+(B27-C27)/C26</f>
         <v>-3.75</v>
@@ -758,7 +820,7 @@
         <v>191.25</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:7">
       <c r="B29" t="s">
         <v>10</v>
       </c>
@@ -766,7 +828,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -775,7 +837,7 @@
         <v>2.8888888888888888</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:7">
       <c r="B32">
         <v>160</v>
       </c>
@@ -785,8 +847,16 @@
       <c r="D32">
         <v>560</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="F32">
+        <f>C32-90*C31</f>
+        <v>135</v>
+      </c>
+      <c r="G32">
+        <f>C32+90*C31</f>
+        <v>655</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="B33">
         <f>90+(B32-C32)/C31</f>
         <v>8.6538461538461462</v>
@@ -799,7 +869,7 @@
         <v>147.11538461538461</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:7">
       <c r="B34" t="s">
         <v>4</v>
       </c>
@@ -807,7 +877,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>17</v>
       </c>
@@ -816,7 +886,7 @@
         <v>3.1111111111111112</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:7">
       <c r="B36">
         <v>160</v>
       </c>
@@ -826,8 +896,16 @@
       <c r="D36">
         <v>460</v>
       </c>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="F36">
+        <f>C36-90*C35</f>
+        <v>-50</v>
+      </c>
+      <c r="G36">
+        <f>C36+90*C35</f>
+        <v>510</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="B37">
         <f>90+(B36-C36)/C35</f>
         <v>67.5</v>
@@ -840,7 +918,7 @@
         <v>163.92857142857144</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:7">
       <c r="B38" t="s">
         <v>14</v>
       </c>
@@ -848,7 +926,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:7">
       <c r="A39" t="s">
         <v>18</v>
       </c>
@@ -857,7 +935,7 @@
         <v>2.8888888888888888</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:7">
       <c r="B40">
         <v>150</v>
       </c>
@@ -867,8 +945,16 @@
       <c r="D40">
         <v>650</v>
       </c>
-    </row>
-    <row r="41" spans="1:4">
+      <c r="F40">
+        <f>C40-90*C39</f>
+        <v>120</v>
+      </c>
+      <c r="G40">
+        <f>C40+90*C39</f>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="B41">
         <f>90+(B40-C40)/C39</f>
         <v>10.384615384615387</v>
@@ -881,7 +967,7 @@
         <v>183.46153846153845</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:7">
       <c r="B42" t="s">
         <v>10</v>
       </c>

</xml_diff>